<commit_message>
Complete task phase 1
</commit_message>
<xml_diff>
--- a/giansalex/evidence.xlsx
+++ b/giansalex/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -97,34 +97,52 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
+    <t xml:space="preserve">48DFB7131C81C51F68AB272A76CE9F719E1F1D40223521DF3FA979D9A621CE16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disperze01</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">nft id you minted</t>
+    <t xml:space="preserve">EF518A526294443C1E69A1C0824B102BD04A61E0CA1E274AC6A7934194033FAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gonft001</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">BDF8620D61C53F47158E6D9DEB9C00EF68BDE52FC963C8D3AC21615D696279C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juno19gumnz9f2we022mkauae3v29jkyf0e5mqwy8ex8p9klav7ntwxfq8wjrcv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC6A13793DD3762C11522E658946FC57C28DD45E53A6B44E4969ACDA4369EAC0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/7A2A1E0D341C654C86538C4D3129DEF3DEBD8CF3F4DE239DDDC2DC21361402D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">516CD98BABEEBACCC6793D4F325F06EBC033269D61B2D3D98A4B6EB431BB0172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0A983C0378B0969F9EE4E314E8274AB8015BFE38561EF24720871EB3BD475B74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -341,16 +359,16 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="16.81"/>
@@ -427,7 +445,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -442,10 +460,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +488,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -485,10 +503,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +531,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -528,10 +546,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -556,7 +574,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -571,10 +589,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -599,7 +617,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -609,25 +627,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +670,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -662,25 +680,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -705,7 +723,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -715,25 +733,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +776,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -768,25 +786,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -811,7 +829,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -821,25 +839,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +882,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -874,25 +892,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -914,53 +932,53 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.89"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -970,25 +988,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1013,7 +1031,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1023,25 +1041,25 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1084,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1075,12 +1093,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1123,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1114,12 +1132,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1144,7 +1162,7 @@
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1153,12 +1171,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1183,7 +1201,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1192,12 +1210,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1219,10 +1237,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1241,13 +1259,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1269,10 +1287,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1289,21 +1307,21 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1325,10 +1343,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1345,21 +1363,21 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1381,10 +1399,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1401,22 +1419,22 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1436,16 +1454,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,21 +1477,21 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1498,7 +1516,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1513,10 +1531,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1541,7 +1559,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1556,10 +1574,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>